<commit_message>
- Updated broken Table Generator tests after previous changes. - Minor changes to Gradle scripts toward supporing building the project without IntelliJ.
</commit_message>
<xml_diff>
--- a/table-generator/src/test/resources/test_data/test_table_with_numeric_id.xlsx
+++ b/table-generator/src/test/resources/test_data/test_table_with_numeric_id.xlsx
@@ -44,10 +44,10 @@
     <t>No</t>
   </si>
   <si>
-    <t>root-code-name.common-code-name-1</t>
-  </si>
-  <si>
-    <t>1:2</t>
+    <t>common-code-name-1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>Message for CName1 error.</t>
@@ -59,19 +59,19 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>root-code-name.common-code-name-1.common-code-name-2</t>
-  </si>
-  <si>
-    <t>1:2:3</t>
+    <t>common-code-name-1.common-code-name-2</t>
+  </si>
+  <si>
+    <t>2:3</t>
   </si>
   <si>
     <t>CName2Exception</t>
   </si>
   <si>
-    <t>root-code-name.common-code-name-1.common-code-name-2.common-code-name-3-1</t>
-  </si>
-  <si>
-    <t>1:2:3:4</t>
+    <t>common-code-name-1.common-code-name-2.common-code-name-3-1</t>
+  </si>
+  <si>
+    <t>2:3:4</t>
   </si>
   <si>
     <t>Message for CName3_1 error.</t>
@@ -80,10 +80,10 @@
     <t>CName3_1Exception</t>
   </si>
   <si>
-    <t>root-code-name.common-code-name-1.common-code-name-2.common-code-name-3-2</t>
-  </si>
-  <si>
-    <t>1:2:3:5</t>
+    <t>common-code-name-1.common-code-name-2.common-code-name-3-2</t>
+  </si>
+  <si>
+    <t>2:3:5</t>
   </si>
   <si>
     <t>CName3_2: {param1: '%s', param2: %d, param3: '%s'}</t>
@@ -92,10 +92,10 @@
     <t>CName3_2Exception</t>
   </si>
   <si>
-    <t>root-code-name.common-code-name-1.common-code-name-2.common-code-name-3-3</t>
-  </si>
-  <si>
-    <t>1:2:3:6</t>
+    <t>common-code-name-1.common-code-name-2.common-code-name-3-3</t>
+  </si>
+  <si>
+    <t>2:3:6</t>
   </si>
   <si>
     <t>TestMessageGeneratorObject1</t>
@@ -104,10 +104,10 @@
     <t>CName3_3Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-code-name-1</t>
-  </si>
-  <si>
-    <t>1:7</t>
+    <t>error-code-name-1</t>
+  </si>
+  <si>
+    <t>7</t>
   </si>
   <si>
     <t>Message for EName1 error.</t>
@@ -116,19 +116,19 @@
     <t>EName1Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-code-name-1.error-code-name-2</t>
-  </si>
-  <si>
-    <t>1:7:8</t>
+    <t>error-code-name-1.error-code-name-2</t>
+  </si>
+  <si>
+    <t>7:8</t>
   </si>
   <si>
     <t>EName2Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-code-name-1.error-code-name-2.error-code-name-3-1</t>
-  </si>
-  <si>
-    <t>1:7:8:9</t>
+    <t>error-code-name-1.error-code-name-2.error-code-name-3-1</t>
+  </si>
+  <si>
+    <t>7:8:9</t>
   </si>
   <si>
     <t>Message for EName3_1 error.</t>
@@ -137,10 +137,10 @@
     <t>EName3_1Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-code-name-1.error-code-name-2.error-code-name-3-2</t>
-  </si>
-  <si>
-    <t>1:7:8:10</t>
+    <t>error-code-name-1.error-code-name-2.error-code-name-3-2</t>
+  </si>
+  <si>
+    <t>7:8:10</t>
   </si>
   <si>
     <t>EName3_2: {param1: '%s', param2: %d, param3: '%s'}</t>
@@ -149,10 +149,10 @@
     <t>EName3_2Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-code-name-1.error-code-name-2.error-code-name-3-3</t>
-  </si>
-  <si>
-    <t>1:7:8:11</t>
+    <t>error-code-name-1.error-code-name-2.error-code-name-3-3</t>
+  </si>
+  <si>
+    <t>7:8:11</t>
   </si>
   <si>
     <t>TestMessageGeneratorObject2</t>
@@ -161,10 +161,10 @@
     <t>EName3_3Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-2-code-name-1</t>
-  </si>
-  <si>
-    <t>1:12</t>
+    <t>error-2-code-name-1</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>Message for E2Name1 error.</t>
@@ -173,19 +173,19 @@
     <t>E2Name1Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-2-code-name-1.error-2-code-name-2</t>
-  </si>
-  <si>
-    <t>1:12:13</t>
+    <t>error-2-code-name-1.error-2-code-name-2</t>
+  </si>
+  <si>
+    <t>12:13</t>
   </si>
   <si>
     <t>E2Name2Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-1</t>
-  </si>
-  <si>
-    <t>1:12:13:14</t>
+    <t>error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-1</t>
+  </si>
+  <si>
+    <t>12:13:14</t>
   </si>
   <si>
     <t>Message for E2Name3_1 error.</t>
@@ -194,10 +194,10 @@
     <t>E2Name3_1Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-2</t>
-  </si>
-  <si>
-    <t>1:12:13:15</t>
+    <t>error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-2</t>
+  </si>
+  <si>
+    <t>12:13:15</t>
   </si>
   <si>
     <t>E2Name3_2: {param1: '%s', param2: %d, param3: '%s'}</t>
@@ -206,10 +206,10 @@
     <t>E2Name3_2Exception</t>
   </si>
   <si>
-    <t>root-code-name.error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-3</t>
-  </si>
-  <si>
-    <t>1:12:13:16</t>
+    <t>error-2-code-name-1.error-2-code-name-2.error-2-code-name-3-3</t>
+  </si>
+  <si>
+    <t>12:13:16</t>
   </si>
   <si>
     <t>TestMessageGeneratorObject3</t>
@@ -320,7 +320,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>